<commit_message>
Planilhas Atualizadas, obs: Pasta 'EVA_PROJETO' vazia?
</commit_message>
<xml_diff>
--- a/1.Administrativo/2.Planilhas/Gerenciamento Projeto PI.xlsx
+++ b/1.Administrativo/2.Planilhas/Gerenciamento Projeto PI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markz\Desktop\eva\1.Administrativo\2.Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7EB73-63D6-4866-8907-06A10B20ABEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5693396B-6740-4A7D-ABEC-550FF9E6F0D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Reuniões!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$G$21</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="53">
   <si>
     <t>Reuniões</t>
   </si>
@@ -162,13 +162,40 @@
   </si>
   <si>
     <t>Banco de Dados</t>
+  </si>
+  <si>
+    <t>1ª</t>
+  </si>
+  <si>
+    <t>DashBoard</t>
+  </si>
+  <si>
+    <t>PowerPoint</t>
+  </si>
+  <si>
+    <t>2ª</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>Regras de Conduta</t>
+  </si>
+  <si>
+    <t>Plano de Ação</t>
+  </si>
+  <si>
+    <t>Dev Master</t>
+  </si>
+  <si>
+    <t>5ª</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,8 +211,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +241,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC348E4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -271,12 +323,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC348E4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -551,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,14 +660,14 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
+      <c r="A2" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>10</v>
@@ -618,8 +684,8 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>1</v>
+      <c r="A3" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -642,8 +708,8 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>1</v>
+      <c r="A4" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
@@ -666,8 +732,8 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>1</v>
+      <c r="A5" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
@@ -690,8 +756,8 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>1</v>
+      <c r="A6" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>8</v>
@@ -714,8 +780,8 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>1</v>
+      <c r="A7" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>9</v>
@@ -738,8 +804,8 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>1</v>
+      <c r="A8" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
@@ -762,8 +828,8 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>1</v>
+      <c r="A9" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
@@ -786,17 +852,17 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>1</v>
+      <c r="A10" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>14</v>
@@ -810,17 +876,17 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>1</v>
+      <c r="A11" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>14</v>
@@ -834,14 +900,14 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>1</v>
+      <c r="A12" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>43</v>
@@ -850,101 +916,223 @@
         <v>14</v>
       </c>
       <c r="F12" s="7">
-        <v>43930</v>
-      </c>
-      <c r="G12" s="11" t="s">
+        <v>43936</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="7">
+        <v>43936</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="7">
+        <v>43936</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="7">
+        <v>43936</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="7">
+        <v>43936</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="A17" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="7">
+        <v>43936</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="A18" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="7">
+        <v>43936</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="7">
+        <v>43959</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="7">
+        <v>43959</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="7">
+        <v>43959</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -967,8 +1155,32 @@
       <c r="G23" s="5"/>
       <c r="H23" s="2"/>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{D29BEDAF-B02F-42B7-8375-C7714A4CB2FF}"/>
+  <autoFilter ref="A1:G21" xr:uid="{D29BEDAF-B02F-42B7-8375-C7714A4CB2FF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -979,7 +1191,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,8 +1229,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
+      <c r="A2" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -1040,8 +1252,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>1</v>
+      <c r="A3" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -1059,8 +1271,8 @@
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>1</v>
+      <c r="A4" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -1078,8 +1290,8 @@
       <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>1</v>
+      <c r="A5" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B5" s="5">
         <v>4</v>
@@ -1101,8 +1313,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>1</v>
+      <c r="A6" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B6" s="5">
         <v>5</v>
@@ -1120,8 +1332,8 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>1</v>
+      <c r="A7" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B7" s="5">
         <v>6</v>

</xml_diff>

<commit_message>
backlog adcionado, planilhas atualizadas
</commit_message>
<xml_diff>
--- a/1.Administrativo/2.Planilhas/Gerenciamento Projeto PI.xlsx
+++ b/1.Administrativo/2.Planilhas/Gerenciamento Projeto PI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markz\Desktop\eva\1.Administrativo\2.Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5693396B-6740-4A7D-ABEC-550FF9E6F0D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAD3333-F63A-4327-BF2B-0839DDB6E031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
   <si>
     <t>Reuniões</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>5ª</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev </t>
+  </si>
+  <si>
+    <t>Backlog parciealmente finalizado</t>
   </si>
 </sst>
 </file>
@@ -619,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1009,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>42</v>
@@ -1092,7 +1098,9 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="B20" s="5" t="s">
         <v>6</v>
       </c>
@@ -1114,7 +1122,9 @@
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="B21" s="5" t="s">
         <v>7</v>
       </c>
@@ -1190,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AEDFE8-CB33-4D46-942E-DD0750198DE8}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="150" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,13 +1361,25 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="7">
+        <v>43924</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
@@ -1533,5 +1555,6 @@
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{1CE7BE42-E684-4898-87B2-2BA7540E6928}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>